<commit_message>
- Se agrega icono de descarga de supervisión en vista editar hoja de vida - Se corrige formato
</commit_message>
<xml_diff>
--- a/IVSoftware.Web/Formats/F-MA-96.xlsx
+++ b/IVSoftware.Web/Formats/F-MA-96.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Preguntas" sheetId="1" r:id="rId1"/>
@@ -602,6 +602,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -610,26 +613,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,9 +626,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,7 +730,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2563,7 +2563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2577,7 +2577,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50"/>
+      <c r="A1" s="27"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2717,12 +2717,12 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="30"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
@@ -2749,12 +2749,12 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2781,12 +2781,12 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
@@ -30721,7 +30721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -30899,19 +30901,19 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="45"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="34"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
@@ -30944,12 +30946,12 @@
       <c r="E8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="48"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
@@ -30971,7 +30973,8 @@
         <v>17</v>
       </c>
       <c r="B9" s="12">
-        <v>6</v>
+        <f>COUNTIFS(Preguntas!$B:$B,Resultados!$A9,Preguntas!$E:$E,Resultados!B$8)</f>
+        <v>0</v>
       </c>
       <c r="C9" s="13">
         <f>COUNTIFS(Preguntas!$B:$B,Resultados!$A9,Preguntas!$E:$E,Resultados!C$8)</f>
@@ -30985,12 +30988,12 @@
         <f>COUNTIFS(Preguntas!$B:$B,Resultados!$A9,Preguntas!$E:$E,Resultados!E$8)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="48"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="37"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -31012,6 +31015,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="12">
+        <f>COUNTIFS(Preguntas!$B:$B,Resultados!$A10,Preguntas!$E:$E,Resultados!B$8)</f>
         <v>0</v>
       </c>
       <c r="C10" s="13">
@@ -31026,12 +31030,12 @@
         <f>COUNTIFS(Preguntas!$B:$B,Resultados!$A10,Preguntas!$E:$E,Resultados!E$8)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="48"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
@@ -31068,12 +31072,12 @@
         <f>COUNTIFS(Preguntas!$B:$B,Resultados!$A11,Preguntas!$E:$E,Resultados!E$8)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="37"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
@@ -31110,12 +31114,12 @@
         <f>COUNTIFS(Preguntas!$B:$B,Resultados!$A12,Preguntas!$E:$E,Resultados!E$8)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="48"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
@@ -31138,12 +31142,12 @@
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="48"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
@@ -31176,12 +31180,12 @@
       <c r="E14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="48"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
@@ -31218,12 +31222,12 @@
         <f>COUNTIFS(Preguntas!$C:$C,Resultados!$A15,Preguntas!$E:$E,Resultados!E$14)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="48"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="37"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
@@ -31260,12 +31264,12 @@
         <f>COUNTIFS(Preguntas!$C:$C,Resultados!$A16,Preguntas!$E:$E,Resultados!E$14)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="48"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="37"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
@@ -31302,12 +31306,12 @@
         <f>COUNTIFS(Preguntas!$C:$C,Resultados!$A17,Preguntas!$E:$E,Resultados!E$14)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="48"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="37"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
@@ -31344,12 +31348,12 @@
         <f>COUNTIFS(Preguntas!$C:$C,Resultados!$A18,Preguntas!$E:$E,Resultados!E$14)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="48"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="37"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
@@ -31386,12 +31390,12 @@
         <f>COUNTIFS(Preguntas!$C:$C,Resultados!$A19,Preguntas!$E:$E,Resultados!E$14)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="48"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="37"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
@@ -31428,12 +31432,12 @@
         <f>COUNTIFS(Preguntas!$C:$C,Resultados!$A20,Preguntas!$E:$E,Resultados!E$14)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="48"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
@@ -31470,12 +31474,12 @@
         <f>COUNTIFS(Preguntas!$C:$C,Resultados!$A21,Preguntas!$E:$E,Resultados!E$14)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="48"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="37"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
@@ -31536,7 +31540,7 @@
       <c r="E23" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="49" t="s">
+      <c r="F23" s="38" t="s">
         <v>30</v>
       </c>
       <c r="G23" s="39"/>
@@ -31581,12 +31585,12 @@
         <f>COUNTIF(Preguntas!H:H,Resultados!E23)/$A$24</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="42"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="43"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
@@ -31632,19 +31636,19 @@
       <c r="Z25" s="7"/>
     </row>
     <row r="26" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="45"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="34"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
@@ -31665,20 +31669,20 @@
       <c r="A27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="33" t="s">
+      <c r="C27" s="45"/>
+      <c r="D27" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="35"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="48"/>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
@@ -31699,9 +31703,9 @@
       <c r="A28" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="36"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
       <c r="G28" s="39"/>
@@ -31729,9 +31733,9 @@
       <c r="A29" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="36"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="49"/>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
       <c r="G29" s="39"/>
@@ -31759,9 +31763,9 @@
       <c r="A30" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="36"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="39"/>
       <c r="F30" s="39"/>
       <c r="G30" s="39"/>
@@ -31789,9 +31793,9 @@
       <c r="A31" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="36"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="39"/>
       <c r="F31" s="39"/>
       <c r="G31" s="39"/>
@@ -31819,9 +31823,9 @@
       <c r="A32" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="39"/>
       <c r="F32" s="39"/>
       <c r="G32" s="39"/>
@@ -31849,16 +31853,16 @@
       <c r="A33" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="42"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="43"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
@@ -58953,11 +58957,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="F8:K21"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="A26:K26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:K27"/>
     <mergeCell ref="B31:C31"/>
@@ -58972,6 +58971,11 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:K30"/>
     <mergeCell ref="D31:K31"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="F8:K21"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="A26:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="64" orientation="portrait"/>

</xml_diff>